<commit_message>
also hormesis index no valid
</commit_message>
<xml_diff>
--- a/data/2024 Imrana-food/2_days.xlsx
+++ b/data/2024 Imrana-food/2_days.xlsx
@@ -496,9 +496,7 @@
       <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="5">
-        <v>1.66666666666667</v>
-      </c>
+      <c r="F4" s="5"/>
       <c r="G4" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">

</xml_diff>